<commit_message>
hid some things, deleted some wrong things
</commit_message>
<xml_diff>
--- a/Behavioral testing/mturk/results/Results_1st_10_only.xlsx
+++ b/Behavioral testing/mturk/results/Results_1st_10_only.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="460" windowWidth="24960" windowHeight="13760" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="24960" windowHeight="13760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OrderA" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="224">
   <si>
     <t>Order presented</t>
   </si>
@@ -461,12 +461,6 @@
   </si>
   <si>
     <t>A happy square stands on a bank and pushes a happy oval into the water. The oval bounces.</t>
-  </si>
-  <si>
-    <t>ASumForVerb</t>
-  </si>
-  <si>
-    <t>PSumForVerb</t>
   </si>
   <si>
     <t>http://tedlab.mit.edu/~mekline/AP062016/Agent_flipped_29.jpg</t>
@@ -1031,11 +1025,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="16" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1101,123 +1100,123 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q2" s="1">
         <v>1</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1">
         <v>1</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
@@ -1225,49 +1224,49 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>5</v>
@@ -1287,49 +1286,49 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>5</v>
@@ -1349,13 +1348,13 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1">
         <v>23</v>
@@ -1364,16 +1363,16 @@
         <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>46</v>
@@ -1385,13 +1384,13 @@
         <v>6</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>5</v>
@@ -1473,49 +1472,49 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D8" s="1">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>5</v>
@@ -1535,46 +1534,46 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>32</v>
@@ -1597,67 +1596,71 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:T10">
+    <sortCondition ref="E2:E10"/>
+    <sortCondition ref="H2:H10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1666,11 +1669,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" activeCellId="4" sqref="C1:C1048576 D1:D1048576 F1:F1048576 G1:G1048576 I1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="16" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1736,122 +1744,122 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>IF(F2=K2,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P2" s="1" t="str">
         <f>IF(F2=O2,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q2" s="1">
         <f>IF(L2="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1">
         <f>IF(P2="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1">
         <f>IF(L2="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="1">
         <f>IF(P2="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF(F3=K3,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P3" s="1" t="str">
         <f>IF(F3=O3,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q3" s="1">
         <f>IF(L3="Agent",1,0)</f>
@@ -1859,7 +1867,7 @@
       </c>
       <c r="R3" s="1">
         <f>IF(P3="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1">
         <f>IF(L3="Patient",1,0)</f>
@@ -1867,7 +1875,7 @@
       </c>
       <c r="T3" s="1">
         <f>IF(P3="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1940,50 +1948,50 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D5" s="1">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L5" s="1" t="str">
         <f>IF(F5=K5,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5" s="1" t="str">
         <f>IF(F5=O5,"Agent","Patient")</f>
@@ -2008,54 +2016,54 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>IF(F6=K6,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P6" s="1" t="str">
         <f>IF(F6=O6,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q6" s="1">
         <f>IF(L6="Agent",1,0)</f>
@@ -2063,7 +2071,7 @@
       </c>
       <c r="R6" s="1">
         <f>IF(P6="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="1">
         <f>IF(L6="Patient",1,0)</f>
@@ -2071,24 +2079,24 @@
       </c>
       <c r="T6" s="1">
         <f>IF(P6="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>44</v>
@@ -2100,10 +2108,10 @@
         <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>23</v>
@@ -2113,17 +2121,17 @@
         <v>Patient</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="P7" s="1" t="str">
         <f>IF(F7=O7,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q7" s="1">
         <f>IF(L7="Agent",1,0)</f>
@@ -2131,7 +2139,7 @@
       </c>
       <c r="R7" s="1">
         <f>IF(P7="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="1">
         <f>IF(L7="Patient",1,0)</f>
@@ -2139,55 +2147,55 @@
       </c>
       <c r="T7" s="1">
         <f>IF(P7="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>IF(F8=K8,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P8" s="1" t="str">
         <f>IF(F8=O8,"Agent","Patient")</f>
@@ -2212,118 +2220,118 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>IF(F9=K9,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="P9" s="1" t="str">
         <f>IF(F9=O9,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q9" s="1">
         <f>IF(L9="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="1">
         <f>IF(P9="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="1">
         <f>IF(L9="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="1">
         <f>IF(P9="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D10" s="1">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="L10" s="1" t="str">
         <f>IF(F10=K10,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P10" s="1" t="str">
         <f>IF(F10=O10,"Agent","Patient")</f>
@@ -2348,54 +2356,54 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>IF(F11=K11,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="P11" s="1" t="str">
         <f>IF(F11=O11,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q11" s="1">
         <f>IF(L11="Agent",1,0)</f>
@@ -2403,7 +2411,7 @@
       </c>
       <c r="R11" s="1">
         <f>IF(P11="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" s="1">
         <f>IF(L11="Patient",1,0)</f>
@@ -2411,10 +2419,14 @@
       </c>
       <c r="T11" s="1">
         <f>IF(P11="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:T11">
+    <sortCondition ref="E2:E11"/>
+    <sortCondition ref="H2:H11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2423,11 +2435,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" activeCellId="3" sqref="A1:D1048576 F1:F1048576 G1:G1048576 I1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="16" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2493,34 +2510,34 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D2" s="1">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -2530,17 +2547,17 @@
         <v>Agent</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="P2" t="str">
         <f>IF(F2=O2,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q2" s="1">
         <f>IF(L2="Agent",1,0)</f>
@@ -2548,7 +2565,7 @@
       </c>
       <c r="R2" s="1">
         <f>IF(P2="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1">
         <f>IF(L2="Patient",1,0)</f>
@@ -2556,123 +2573,123 @@
       </c>
       <c r="T2" s="1">
         <f>IF(P2="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D3" s="1">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF(F3=K3,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P3" t="str">
         <f>IF(F3=O3,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q3" s="1">
         <f>IF(L3="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1">
         <f>IF(P3="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="1">
         <f>IF(L3="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1">
         <f>IF(P3="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="D4" s="1">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>IF(F4=K4,"Agent","Patient")</f>
         <v>Agent</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="P4" t="str">
         <f>IF(F4=O4,"Agent","Patient")</f>
@@ -2697,34 +2714,34 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>24</v>
@@ -2734,10 +2751,10 @@
         <v>Agent</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>24</v>
@@ -2765,50 +2782,50 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>IF(F6=K6,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="P6" t="str">
         <f>IF(F6=O6,"Agent","Patient")</f>
@@ -2816,7 +2833,7 @@
       </c>
       <c r="Q6" s="1">
         <f>IF(L6="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="1">
         <f>IF(P6="Agent",1,0)</f>
@@ -2824,7 +2841,7 @@
       </c>
       <c r="S6" s="1">
         <f>IF(L6="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1">
         <f>IF(P6="Patient",1,0)</f>
@@ -2901,19 +2918,19 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
@@ -2922,26 +2939,26 @@
         <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>133</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>IF(F8=K8,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>24</v>
@@ -2952,7 +2969,7 @@
       </c>
       <c r="Q8" s="1">
         <f>IF(L8="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1">
         <f>IF(P8="Agent",1,0)</f>
@@ -2960,7 +2977,7 @@
       </c>
       <c r="S8" s="1">
         <f>IF(L8="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1">
         <f>IF(P8="Patient",1,0)</f>
@@ -2969,50 +2986,50 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>IF(F9=K9,"Agent","Patient")</f>
         <v>Agent</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P9" t="str">
         <f>IF(F9=O9,"Agent","Patient")</f>
@@ -3105,47 +3122,47 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>IF(F11=K11,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>24</v>
@@ -3156,7 +3173,7 @@
       </c>
       <c r="Q11" s="1">
         <f>IF(L11="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11" s="1">
         <f>IF(P11="Agent",1,0)</f>
@@ -3164,7 +3181,7 @@
       </c>
       <c r="S11" s="1">
         <f>IF(L11="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="1">
         <f>IF(P11="Patient",1,0)</f>
@@ -3172,21 +3189,31 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:T11">
+    <sortCondition ref="E2:E11"/>
+    <sortCondition ref="H2:H11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3247,14 +3274,8 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
-        <v>144</v>
-      </c>
-      <c r="V1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -3262,7 +3283,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="1">
         <v>29</v>
@@ -3280,7 +3301,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>95</v>
@@ -3293,10 +3314,10 @@
         <v>Patient</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>24</v>
@@ -3322,52 +3343,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF(F3=K3,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P3" t="str">
         <f>IF(F3=O3,"Agent","Patient")</f>
@@ -3375,7 +3396,7 @@
       </c>
       <c r="Q3">
         <f>IF(L3="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <f>IF(P3="Agent",1,0)</f>
@@ -3383,99 +3404,96 @@
       </c>
       <c r="S3">
         <f>IF(L3="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <f>IF(P3="Patient",1,0)</f>
         <v>1</v>
       </c>
-      <c r="U3">
-        <f>SUM(Q3:R26)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
+        <v>160</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>IF(F4=K4,"Agent","Patient")</f>
+        <v>Patient</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" t="str">
+        <f>IF(F4=O4,"Agent","Patient")</f>
         <v>Agent</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P4" t="s">
-        <v>157</v>
       </c>
       <c r="Q4">
         <f>IF(L4="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <f>IF(P4="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <f>IF(L4="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
         <f>IF(P4="Patient",1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D5" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -3484,13 +3502,13 @@
         <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>24</v>
@@ -3500,17 +3518,17 @@
         <v>Agent</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P5" t="str">
         <f>IF(F5=O5,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q5">
         <f>IF(L5="Agent",1,0)</f>
@@ -3518,7 +3536,7 @@
       </c>
       <c r="R5">
         <f>IF(P5="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f>IF(L5="Patient",1,0)</f>
@@ -3526,78 +3544,77 @@
       </c>
       <c r="T5">
         <f>IF(P5="Patient",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="D6" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>IF(F6=K6,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" t="str">
-        <f>IF(F6=O6,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>155</v>
+      </c>
+      <c r="P6" t="s">
+        <v>155</v>
       </c>
       <c r="Q6">
         <f>IF(L6="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f>IF(P6="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
         <f>IF(L6="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <f>IF(P6="Patient",1,0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -3623,7 +3640,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>31</v>
@@ -3636,7 +3653,7 @@
         <v>Agent</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>31</v>
@@ -3665,52 +3682,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="1">
-        <v>18</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>IF(F8=K8,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="P8" t="str">
         <f>IF(F8=O8,"Agent","Patient")</f>
@@ -3718,7 +3735,7 @@
       </c>
       <c r="Q8">
         <f>IF(L8="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f>IF(P8="Agent",1,0)</f>
@@ -3726,28 +3743,28 @@
       </c>
       <c r="S8">
         <f>IF(L8="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <f>IF(P8="Patient",1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="D9" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
@@ -3756,52 +3773,52 @@
         <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>IF(F9=K9,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P9" t="str">
         <f>IF(F9=O9,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q9">
         <f>IF(L9="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f>IF(P9="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f>IF(L9="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <f>IF(P9="Patient",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>65</v>
       </c>
@@ -3809,7 +3826,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1">
         <v>40</v>
@@ -3827,7 +3844,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>22</v>
@@ -3840,7 +3857,7 @@
         <v>Agent</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>125</v>
@@ -3869,49 +3886,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="D11" s="1">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>IF(F11=K11,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>23</v>
@@ -3922,7 +3939,7 @@
       </c>
       <c r="Q11">
         <f>IF(L11="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11">
         <f>IF(P11="Agent",1,0)</f>
@@ -3930,7 +3947,7 @@
       </c>
       <c r="S11">
         <f>IF(L11="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
         <f>IF(P11="Patient",1,0)</f>
@@ -3938,6 +3955,10 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:V11">
+    <sortCondition ref="E2:E11"/>
+    <sortCondition ref="H2:H11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3947,7 +3968,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4016,19 +4037,19 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="D2" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
@@ -4040,23 +4061,23 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>IF(F2=K2,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>32</v>
@@ -4067,7 +4088,7 @@
       </c>
       <c r="Q2" s="1">
         <f>IF(L2="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="1">
         <f>IF(P2="Agent",1,0)</f>
@@ -4075,7 +4096,7 @@
       </c>
       <c r="S2" s="1">
         <f>IF(L2="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="1">
         <f>IF(P2="Patient",1,0)</f>
@@ -4084,118 +4105,118 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D3" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="1" t="str">
         <f>IF(F3=K3,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P3" t="str">
         <f>IF(F3=O3,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q3" s="1">
         <f>IF(L3="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1">
         <f>IF(P3="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" s="1">
         <f>IF(L3="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="1">
         <f>IF(P3="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="D4" s="1">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>IF(F4=K4,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>127</v>
+        <v>206</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="P4" t="str">
         <f>IF(F4=O4,"Agent","Patient")</f>
@@ -4220,122 +4241,122 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="str">
         <f>IF(F5=K5,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="P5" t="str">
         <f>IF(F5=O5,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q5" s="1">
         <f>IF(L5="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5" s="1">
         <f>IF(P5="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
         <f>IF(L5="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="1">
         <f>IF(P5="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D6" s="1">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L6" s="1" t="str">
         <f>IF(F6=K6,"Agent","Patient")</f>
         <v>Patient</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="P6" t="str">
         <f>IF(F6=O6,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="Q6" s="1">
         <f>IF(L6="Agent",1,0)</f>
@@ -4343,7 +4364,7 @@
       </c>
       <c r="R6" s="1">
         <f>IF(P6="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" s="1">
         <f>IF(L6="Patient",1,0)</f>
@@ -4351,39 +4372,39 @@
       </c>
       <c r="T6" s="1">
         <f>IF(P6="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D7" s="1">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>180</v>
+        <v>68</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>32</v>
@@ -4393,10 +4414,10 @@
         <v>Patient</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>32</v>
@@ -4424,99 +4445,99 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="D8" s="1">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>IF(F8=K8,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="P8" t="str">
         <f>IF(F8=O8,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q8" s="1">
         <f>IF(L8="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="1">
         <f>IF(P8="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="1">
         <f>IF(L8="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1">
         <f>IF(P8="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D9" s="1">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>26</v>
@@ -4526,16 +4547,16 @@
       </c>
       <c r="L9" s="1" t="str">
         <f>IF(F9=K9,"Agent","Patient")</f>
-        <v>Agent</v>
+        <v>Patient</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>72</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P9" t="str">
         <f>IF(F9=O9,"Agent","Patient")</f>
@@ -4543,7 +4564,7 @@
       </c>
       <c r="Q9" s="1">
         <f>IF(L9="Agent",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" s="1">
         <f>IF(P9="Agent",1,0)</f>
@@ -4551,7 +4572,7 @@
       </c>
       <c r="S9" s="1">
         <f>IF(L9="Patient",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="1">
         <f>IF(P9="Patient",1,0)</f>
@@ -4560,122 +4581,122 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D10" s="1">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>187</v>
+        <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="L10" s="1" t="str">
         <f>IF(F10=K10,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P10" t="str">
         <f>IF(F10=O10,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q10" s="1">
         <f>IF(L10="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="1">
         <f>IF(P10="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="1">
         <f>IF(L10="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="1">
         <f>IF(P10="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D11" s="1">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>IF(F11=K11,"Agent","Patient")</f>
         <v>Agent</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P11" t="str">
         <f>IF(F11=O11,"Agent","Patient")</f>
-        <v>Patient</v>
+        <v>Agent</v>
       </c>
       <c r="Q11" s="1">
         <f>IF(L11="Agent",1,0)</f>
@@ -4683,7 +4704,7 @@
       </c>
       <c r="R11" s="1">
         <f>IF(P11="Agent",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="1">
         <f>IF(L11="Patient",1,0)</f>
@@ -4691,10 +4712,14 @@
       </c>
       <c r="T11" s="1">
         <f>IF(P11="Patient",1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:T11">
+    <sortCondition ref="E2:E11"/>
+    <sortCondition ref="H2:H11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4703,66 +4728,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" t="s">
         <v>212</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>213</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>214</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>215</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>216</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>217</v>
-      </c>
-      <c r="G1" t="s">
-        <v>218</v>
-      </c>
-      <c r="H1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated time points and max time to show events; clarified optseq2 input
also the .DS_store stuff is showing up, but I haven’t noticed any
issues involving it yet so I’ll leave it alone
</commit_message>
<xml_diff>
--- a/Behavioral testing/mturk/results/Results_1st_10_only.xlsx
+++ b/Behavioral testing/mturk/results/Results_1st_10_only.xlsx
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="E1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4771,8 +4771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>